<commit_message>
updated ERD file to match color coding, added data dictionary with color codings and additional metadata fields
</commit_message>
<xml_diff>
--- a/NYPL-menus/ColumnDescriptions.xlsx
+++ b/NYPL-menus/ColumnDescriptions.xlsx
@@ -5,16 +5,20 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Illinois\CS 513\Project\CS513-Project\NYPL-menus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6880ced5148aa379/Desktop/Courses/UIUC/CS513 - Theory and Practice of Data Cleaning/Project/repo/CS513-Project/NYPL-menus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1B393EF3-E6A2-443E-9B9F-B909FE5457F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="113" documentId="8_{1B393EF3-E6A2-443E-9B9F-B909FE5457F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{27C52A45-E8C2-4BE5-A328-452697A551CF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CD750092-602D-475B-9FF4-08BDF5BE9FC9}"/>
+    <workbookView xWindow="38280" yWindow="2700" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CD750092-602D-475B-9FF4-08BDF5BE9FC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Dictionary Format" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Data Dictionary Format'!$A$1:$K$46</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="132">
   <si>
     <t>Column label</t>
   </si>
@@ -387,6 +391,51 @@
   </si>
   <si>
     <t>Dish.csv</t>
+  </si>
+  <si>
+    <t>Schema</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>is_primary_key</t>
+  </si>
+  <si>
+    <t>is_foreign_key</t>
+  </si>
+  <si>
+    <t>Dish</t>
+  </si>
+  <si>
+    <t>NYPL</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>Menu</t>
+  </si>
+  <si>
+    <t>MenuItem</t>
+  </si>
+  <si>
+    <t>MenuPage</t>
+  </si>
+  <si>
+    <t>foreign_key_relationship</t>
+  </si>
+  <si>
+    <t>[MenuPage].[Id]</t>
+  </si>
+  <si>
+    <t>[Dish].[Id]</t>
+  </si>
+  <si>
+    <t>[Menu].[Id]</t>
   </si>
 </sst>
 </file>
@@ -410,15 +459,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -441,11 +514,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -455,6 +539,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -791,8 +882,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDBB67C-A4C1-495C-8D72-DE44B060FFD6}">
   <dimension ref="A1:F56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49:F56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1751,4 +1842,1437 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E50D53-6BC1-42F6-A537-E8067C9A072A}">
+  <dimension ref="A1:K46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="5"/>
+    <col min="2" max="2" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="66" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="255.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K14" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K16" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K18" s="5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K21" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K22" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K23" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K25" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K34" s="5" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="I35" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I36" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K38" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I39" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I40" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D41" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="I41" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K41" s="5" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J43" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B45" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J45" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="I46" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J46" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K46" xr:uid="{C4E50D53-6BC1-42F6-A537-E8067C9A072A}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>